<commit_message>
Muitos ajustes em todo o projeto
</commit_message>
<xml_diff>
--- a/carregar dados/correcao_cotas.xlsx
+++ b/carregar dados/correcao_cotas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monar\Desktop\Programas meus\Python\2025\NotasEnem\carregar dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{36B5D73B-90FA-4230-900F-A8D1CE172CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C7F326-E39A-4508-9AD0-AF71ED02DC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="0" windowWidth="14520" windowHeight="15705" xr2:uid="{9F973CA9-80AA-4E82-A0AE-AC236C219A24}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F973CA9-80AA-4E82-A0AE-AC236C219A24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="231">
   <si>
     <t>Candidato (s) deficientes auditivos especificamente no curso de Letras-Libras.</t>
   </si>
@@ -391,114 +391,6 @@
     <t>Candidato (s) com deficiência</t>
   </si>
   <si>
-    <t>I_PCD_Audio</t>
-  </si>
-  <si>
-    <t>I_PP_EP</t>
-  </si>
-  <si>
-    <t>I_PP</t>
-  </si>
-  <si>
-    <t>I_EP</t>
-  </si>
-  <si>
-    <t>I_PCD</t>
-  </si>
-  <si>
-    <t>I_AF</t>
-  </si>
-  <si>
-    <t>I_I</t>
-  </si>
-  <si>
-    <t>I_PEP</t>
-  </si>
-  <si>
-    <t>B_EP</t>
-  </si>
-  <si>
-    <t>B_PPI</t>
-  </si>
-  <si>
-    <t>B_PCD/FP</t>
-  </si>
-  <si>
-    <t>I_PCD_EP</t>
-  </si>
-  <si>
-    <t>I_I_EP</t>
-  </si>
-  <si>
-    <t>I_EP_EP</t>
-  </si>
-  <si>
-    <t>B_PPI_EP</t>
-  </si>
-  <si>
-    <t>I_PPI_EP</t>
-  </si>
-  <si>
-    <t>I_T_EP</t>
-  </si>
-  <si>
-    <t>I_PPI</t>
-  </si>
-  <si>
-    <t>B_T_EP</t>
-  </si>
-  <si>
-    <t>I_T</t>
-  </si>
-  <si>
-    <t>I_PR</t>
-  </si>
-  <si>
-    <t>I_R</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>I_Q</t>
-  </si>
-  <si>
-    <t>B_Q_EP</t>
-  </si>
-  <si>
-    <t>B_I_EP</t>
-  </si>
-  <si>
-    <t>B_C_EP</t>
-  </si>
-  <si>
-    <t>B_PCD_EP</t>
-  </si>
-  <si>
-    <t>I_IQ_EP</t>
-  </si>
-  <si>
-    <t>B_PP_EP</t>
-  </si>
-  <si>
-    <t>I_Q_EP</t>
-  </si>
-  <si>
-    <t>I_C_EP</t>
-  </si>
-  <si>
-    <t>I_PV_EP</t>
-  </si>
-  <si>
-    <t>I_PFEP</t>
-  </si>
-  <si>
-    <t>I_C</t>
-  </si>
-  <si>
-    <t>I_EFA</t>
-  </si>
-  <si>
     <t>Nome</t>
   </si>
   <si>
@@ -550,9 +442,6 @@
     <t>com deficiência</t>
   </si>
   <si>
-    <t>B_IQ</t>
-  </si>
-  <si>
     <t>Candidatos com deficiência, qualquer que seja a sua procedência escolar.</t>
   </si>
   <si>
@@ -580,12 +469,6 @@
     <t>Pessoas com deficiência, em conformidade com a Lei Estadual nº 20.443, de 17 de dezembro de 2020, que dispõe sobre o ingresso de pessoas com deficiência nas instituições estaduais de educação superior, e não estejam matriculados ou tenham concluído curso superior.  As deficiências para o direito às vagas, segundo Decreto nº 5.296/2004, Lei Federal nº 12.764/2012 e Lei Federal nº 14.126/2021, estão dispostas no endereço https://www3.unicentro.br/vestibular/sisu/cotas-pcd/</t>
   </si>
   <si>
-    <t>B_R</t>
-  </si>
-  <si>
-    <t>B_T</t>
-  </si>
-  <si>
     <t>que tenham cursado integralmente o Ensino Médio em escolas públicas;</t>
   </si>
   <si>
@@ -596,6 +479,240 @@
   </si>
   <si>
     <t>pretos e pardos, que tenham cursado integralmente o Ensino Médio em escolas públicas;</t>
+  </si>
+  <si>
+    <t>VI_PCD_Audio</t>
+  </si>
+  <si>
+    <t>VI_PCD</t>
+  </si>
+  <si>
+    <t>VI_PP</t>
+  </si>
+  <si>
+    <t>VI_EP</t>
+  </si>
+  <si>
+    <t>VI_I</t>
+  </si>
+  <si>
+    <t>VI_PP_EP</t>
+  </si>
+  <si>
+    <t>VI_PEP</t>
+  </si>
+  <si>
+    <t>VI_AF</t>
+  </si>
+  <si>
+    <t>VB_EP</t>
+  </si>
+  <si>
+    <t>VB_PCD/FP</t>
+  </si>
+  <si>
+    <t>VB_PPI</t>
+  </si>
+  <si>
+    <t>VI_I_EP</t>
+  </si>
+  <si>
+    <t>VI_PCD_EP</t>
+  </si>
+  <si>
+    <t>VB_PPI_EP</t>
+  </si>
+  <si>
+    <t>VI_PPI_EP</t>
+  </si>
+  <si>
+    <t>VI_T_EP</t>
+  </si>
+  <si>
+    <t>VI_PPI</t>
+  </si>
+  <si>
+    <t>VB_T_EP</t>
+  </si>
+  <si>
+    <t>VB_T</t>
+  </si>
+  <si>
+    <t>VI_T</t>
+  </si>
+  <si>
+    <t>VI_PR</t>
+  </si>
+  <si>
+    <t>VI_R</t>
+  </si>
+  <si>
+    <t>VB</t>
+  </si>
+  <si>
+    <t>VI_Q</t>
+  </si>
+  <si>
+    <t>VB_Q_EP</t>
+  </si>
+  <si>
+    <t>VB_I_EP</t>
+  </si>
+  <si>
+    <t>VB_C_EP</t>
+  </si>
+  <si>
+    <t>VB_PCD_EP</t>
+  </si>
+  <si>
+    <t>VI_IQ_EP</t>
+  </si>
+  <si>
+    <t>VB_PP_EP</t>
+  </si>
+  <si>
+    <t>VI_Q_EP</t>
+  </si>
+  <si>
+    <t>VI_C_EP</t>
+  </si>
+  <si>
+    <t>VI_PV_EP</t>
+  </si>
+  <si>
+    <t>VI_PFEP</t>
+  </si>
+  <si>
+    <t>VI_C</t>
+  </si>
+  <si>
+    <t>VB_IQ</t>
+  </si>
+  <si>
+    <t>VB_R</t>
+  </si>
+  <si>
+    <t>VI_EFA</t>
+  </si>
+  <si>
+    <t>com Deficiência, Transtorno do Espectro Autista, Altas Habilidades/Superdotação e/ou estudantes que sejam público alvo da educação especial.</t>
+  </si>
+  <si>
+    <t>Candidatos com deficiência (ampla concorrência - Resolução nº 05/2017-CONSUP/IFRN)</t>
+  </si>
+  <si>
+    <t>A2 - Carente Socioeconômico e Negros/Indígenas ou alunos oriundos de Comunidades Quilombolas</t>
+  </si>
+  <si>
+    <t>A3 - Carente Socioeconômico e oriundo da Rede Pública de ensino</t>
+  </si>
+  <si>
+    <t>Candidato (s) que tenham cursado todo o Ensino Médio e os últimos quatro anos do Ensino Fundamental em Escola Pública  e que não se autodeclararam negros.</t>
+  </si>
+  <si>
+    <t>Candidato (s) que tenham cursado todo o Ensino Médio e os últimos quatro anos do Ensino Fundamental em Escola Pública e que se autodeclararam negros.</t>
+  </si>
+  <si>
+    <t>Residentes em Mato Grosso do Sul</t>
+  </si>
+  <si>
+    <t>Quilombola</t>
+  </si>
+  <si>
+    <t>Candidatos professores em exercício do magistério da Pré-Escola, do Ensino Fundamental e Médio da rede pública se ensino.</t>
+  </si>
+  <si>
+    <t>Candidatos A3 - Carente Socioeconômico e da Rede Pública</t>
+  </si>
+  <si>
+    <t>Candidato (s) Indígenas</t>
+  </si>
+  <si>
+    <t>Candidato (s) Quilombolas</t>
+  </si>
+  <si>
+    <t>com deficiência, oriundos de qualquer percurso escolar.</t>
+  </si>
+  <si>
+    <t>Candidato (s) que tenham cursado integralmente o Ensino Médio em instituições públicas e gratuitas de ensino</t>
+  </si>
+  <si>
+    <t>Candidato (s) negros, entendidos como candidatos que possuem fenótipo que os caracterizem, na sociedade, como pertencentes ao grupo racial negro</t>
+  </si>
+  <si>
+    <t>Candidato (s) que tenham cursado na rede pública todo o ensino médio e com comprovação de carência socioeconômica</t>
+  </si>
+  <si>
+    <t>Candidato (s) negros, indígenas ou quilombolas com comprovação de carência socioeconômica</t>
+  </si>
+  <si>
+    <t>Surdos</t>
+  </si>
+  <si>
+    <t>PPI - Cota Social - Pretos, Pardos ou Indígenas</t>
+  </si>
+  <si>
+    <t>PcD - Pessoa com Deficiência</t>
+  </si>
+  <si>
+    <t>EEP - Cota Social - Egressos Escola Pública</t>
+  </si>
+  <si>
+    <t>autodeclarados pretos ou pardos, com renda familiar bruta per capita igual ou inferior a 1,5 salários mínimo que tenham cursado integralmente o ensino médio em escolas públicas (Resolução CONSEPE nº 5.668/2023)</t>
+  </si>
+  <si>
+    <t>Candidato (s) Oriundos da rede pública de ensino.</t>
+  </si>
+  <si>
+    <t>Vagas para PcD</t>
+  </si>
+  <si>
+    <t>Pessoas com deficiência, em conformidade com a Lei Estadual nº 20.443, de 17 de dezembro de 2020, que dispõe sobre o ingresso de pessoas com deficiência nas instituições estaduais de educação superior, e não tenham concluído curso superior.</t>
+  </si>
+  <si>
+    <t>transexuais, travestis e transgêneros que tenham cursado todo o 2º Ciclo do Ensino Fundamental e o Ensino Médio exclusivamente em escola pública, que tenham renda bruta familiar mensal inferior ou igual a 04 (quatro) vezes o valor do salário mínimo nacional vigente no ato da matrícula e que não possuam título de graduação.</t>
+  </si>
+  <si>
+    <t>com deficiência, transtorno do espectro autista e altas habilidades que tenham cursado todo o 2º Ciclo do Ensino Fundamental e o Ensino Médio exclusivamente em escola pública, que tenham renda bruta familiar mensal inferior ou igual a 04 (quatro) vezes o valor do salário mínimo nacional vigente no ato da matrícula e que não possuam título de graduação.</t>
+  </si>
+  <si>
+    <t>A1 - Carente Socioeconômico e Pessoa com Deficiência - PcD ou Carente Socioeconômico e filho(a) de Policiais Civis, Militares, Bombeiros Militares e de Inspetores de Segurança e Administração Penitenciária, Mortos ou Incapacitados em Razão do Serviço</t>
+  </si>
+  <si>
+    <t>Candidato (s) que tenham cursado todo o Ensino Médio e os últimos quatro anos do Ensino Fundamental em Escola Pública e que sejam índios reconhecidos pela FUNAI ou moradores de comunidades remanescentes de quilombos registrados na Fundação Cultural Palmares.</t>
+  </si>
+  <si>
+    <t>Candidatos A1 - Carente Socioeconômico e Pessoa com Deficiência - PcD ou Pessoas Carentes Socioeconômicos e filhos de Policiais Civis, Militares, Bombeiros Militares e de Inspetores de Segurança e Administração Penitenciária, Mortos ou Incapacitados em Razão do Serviço</t>
+  </si>
+  <si>
+    <t>que comprovem ter cursado e concluído todo o Ensino Médio, na forma regular ou técnico-profissionalizante, em escola (s) pública (s) ou privada (s) localizada (s) em município (s) baiano (s) distante (s) até 150 quilômetros de qualquer campus da Universidade Federal do Oeste da Bahia - UFOB.</t>
+  </si>
+  <si>
+    <t>- Candidato (s) com deficiência, ou filhos de policiais civis, militares, bombeiros militares e inspetores de segurança e administração penitenciária, mortos ou incapacitados em razão do serviço, com comprovação de carência socioeconômica</t>
+  </si>
+  <si>
+    <t>que tenham cursado integralmente o ensino médio em escolas públicas, autodeclarados pretos, pardos ou indígenas, nos termos da legislação, que comprovem ser oriundos de famílias com renda igual ou inferior a 1 (um) salário-mínimo per capita.</t>
+  </si>
+  <si>
+    <t>que tenham cursado integralmente o ensino médio em escolas públicas, autodeclarados pretos, pardos ou indígenas, nos termos da legislação, que não declarem ser oriundos de famílias com renda igual ou inferior a 1 (um) salário-mínimo per capita.</t>
+  </si>
+  <si>
+    <t>que tenham cursado integralmente o ensino médio em escolas públicas, que não tenham se declarado pretos, pardos ou indígenas, nos termos da legislação, e que comprovem ser oriundos de famílias com renda igual ou inferior a 1 (um) salário-mínimo per capita.</t>
+  </si>
+  <si>
+    <t>que tenham cursado integralmente o ensino médio em escolas públicas, que não tenham se declarado pretos, pardos ou indígenas, nos termos da legislação, que não declarem ser oriundos de famílias com renda igual ou inferior a 1 (um) salário-mínimo per capita.</t>
+  </si>
+  <si>
+    <t>Candidatos egressos de escolas públicas da rede federal, estadual ou municipal, que cursaram os anos finais do Ensino Fundamental (6º ao 9º anos) e todo o Ensino Médio (1º ao 3º anos), com qualquer renda renda per capita bruta, devendo essa condição ser comprovada no ato da matrícula.</t>
+  </si>
+  <si>
+    <t>Candidatos egressos de escolas públicas da rede federal, estadual ou municipal, que cursaram os anos finais do Ensino Fundamental (6º ao 9º anos) e todo o Ensino Médio (1º ao 3º anos), com renda familiar bruta per capita igual ou inferior a 1,5 salário mínimo, devendo essa condição ser comprovada no ato da matrícula.</t>
+  </si>
+  <si>
+    <t>VI_RG</t>
+  </si>
+  <si>
+    <t>VI_PCD/FP</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1204,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1097,6 +1214,9 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1453,29 +1573,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8613C1C1-16C6-4B43-A738-E2F9C91E29F2}">
-  <dimension ref="A1:B157"/>
+  <dimension ref="A1:B191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B130" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="188.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="132.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -1483,7 +1603,7 @@
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -1491,7 +1611,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -1499,7 +1619,7 @@
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -1507,7 +1627,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -1515,7 +1635,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -1523,7 +1643,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
@@ -1531,7 +1651,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
@@ -1539,7 +1659,7 @@
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
@@ -1547,7 +1667,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
@@ -1555,7 +1675,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>10</v>
@@ -1563,7 +1683,7 @@
     </row>
     <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>11</v>
@@ -1571,7 +1691,7 @@
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
@@ -1579,7 +1699,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
@@ -1587,7 +1707,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>14</v>
@@ -1595,7 +1715,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>134</v>
+        <v>165</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>15</v>
@@ -1603,7 +1723,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>16</v>
@@ -1611,7 +1731,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>17</v>
@@ -1619,7 +1739,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>18</v>
@@ -1627,7 +1747,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>19</v>
@@ -1635,23 +1755,23 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>191</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>20</v>
@@ -1659,7 +1779,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>21</v>
@@ -1667,7 +1787,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>22</v>
@@ -1675,7 +1795,7 @@
     </row>
     <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>23</v>
@@ -1683,7 +1803,7 @@
     </row>
     <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>24</v>
@@ -1691,7 +1811,7 @@
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>25</v>
@@ -1699,7 +1819,7 @@
     </row>
     <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>26</v>
@@ -1707,7 +1827,7 @@
     </row>
     <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>27</v>
@@ -1715,7 +1835,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>28</v>
@@ -1723,7 +1843,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>29</v>
@@ -1731,7 +1851,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>140</v>
+        <v>169</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>30</v>
@@ -1739,7 +1859,7 @@
     </row>
     <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>31</v>
@@ -1747,7 +1867,7 @@
     </row>
     <row r="36" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>32</v>
@@ -1755,7 +1875,7 @@
     </row>
     <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>33</v>
@@ -1763,7 +1883,7 @@
     </row>
     <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>34</v>
@@ -1771,7 +1891,7 @@
     </row>
     <row r="39" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>35</v>
@@ -1779,7 +1899,7 @@
     </row>
     <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>36</v>
@@ -1787,7 +1907,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>37</v>
@@ -1795,7 +1915,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>38</v>
@@ -1803,7 +1923,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>39</v>
@@ -1811,7 +1931,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>143</v>
+        <v>173</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>40</v>
@@ -1819,7 +1939,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>41</v>
@@ -1827,7 +1947,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>42</v>
@@ -1835,7 +1955,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>43</v>
@@ -1843,7 +1963,7 @@
     </row>
     <row r="48" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>44</v>
@@ -1851,7 +1971,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>140</v>
+        <v>169</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>45</v>
@@ -1859,7 +1979,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>46</v>
@@ -1867,7 +1987,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>47</v>
@@ -1875,7 +1995,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>145</v>
+        <v>175</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>48</v>
@@ -1883,7 +2003,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>140</v>
+        <v>169</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>49</v>
@@ -1891,7 +2011,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>50</v>
@@ -1899,7 +2019,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>51</v>
@@ -1907,7 +2027,7 @@
     </row>
     <row r="56" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>52</v>
@@ -1915,7 +2035,7 @@
     </row>
     <row r="57" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>53</v>
@@ -1923,7 +2043,7 @@
     </row>
     <row r="58" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>54</v>
@@ -1931,7 +2051,7 @@
     </row>
     <row r="59" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>55</v>
@@ -1939,7 +2059,7 @@
     </row>
     <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>56</v>
@@ -1947,7 +2067,7 @@
     </row>
     <row r="61" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>57</v>
@@ -1955,7 +2075,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>58</v>
@@ -1963,7 +2083,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>59</v>
@@ -1971,7 +2091,7 @@
     </row>
     <row r="64" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>151</v>
+        <v>181</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>60</v>
@@ -1979,7 +2099,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>61</v>
@@ -1987,7 +2107,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>62</v>
@@ -1995,7 +2115,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>134</v>
+        <v>165</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>63</v>
@@ -2003,7 +2123,7 @@
     </row>
     <row r="68" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>64</v>
@@ -2011,7 +2131,7 @@
     </row>
     <row r="69" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>65</v>
@@ -2019,7 +2139,7 @@
     </row>
     <row r="70" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>66</v>
@@ -2027,7 +2147,7 @@
     </row>
     <row r="71" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>67</v>
@@ -2035,7 +2155,7 @@
     </row>
     <row r="72" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>68</v>
@@ -2043,7 +2163,7 @@
     </row>
     <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>69</v>
@@ -2051,7 +2171,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>153</v>
+        <v>183</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>70</v>
@@ -2059,7 +2179,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>71</v>
@@ -2067,7 +2187,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>72</v>
@@ -2075,7 +2195,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>154</v>
+        <v>184</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>73</v>
@@ -2083,7 +2203,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>74</v>
@@ -2091,7 +2211,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>75</v>
@@ -2099,7 +2219,7 @@
     </row>
     <row r="80" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>76</v>
@@ -2107,7 +2227,7 @@
     </row>
     <row r="81" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>77</v>
@@ -2115,7 +2235,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>156</v>
+        <v>186</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>78</v>
@@ -2123,7 +2243,7 @@
     </row>
     <row r="83" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>79</v>
@@ -2131,7 +2251,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>80</v>
@@ -2139,7 +2259,7 @@
     </row>
     <row r="85" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>81</v>
@@ -2147,7 +2267,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>82</v>
@@ -2155,7 +2275,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>83</v>
@@ -2163,7 +2283,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>84</v>
@@ -2171,7 +2291,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>85</v>
@@ -2179,7 +2299,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>86</v>
@@ -2187,7 +2307,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>87</v>
@@ -2195,7 +2315,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>88</v>
@@ -2203,7 +2323,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>89</v>
@@ -2211,7 +2331,7 @@
     </row>
     <row r="94" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>90</v>
@@ -2219,7 +2339,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>157</v>
+        <v>187</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>91</v>
@@ -2227,7 +2347,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>92</v>
@@ -2235,7 +2355,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>93</v>
@@ -2243,7 +2363,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>94</v>
@@ -2251,7 +2371,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>140</v>
+        <v>169</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>95</v>
@@ -2259,7 +2379,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>96</v>
@@ -2267,7 +2387,7 @@
     </row>
     <row r="101" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>97</v>
@@ -2275,7 +2395,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>134</v>
+        <v>165</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>98</v>
@@ -2283,7 +2403,7 @@
     </row>
     <row r="103" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>99</v>
@@ -2291,7 +2411,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>100</v>
@@ -2299,7 +2419,7 @@
     </row>
     <row r="105" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>101</v>
@@ -2307,7 +2427,7 @@
     </row>
     <row r="106" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>102</v>
@@ -2315,7 +2435,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>103</v>
@@ -2323,7 +2443,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>104</v>
@@ -2331,7 +2451,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>105</v>
@@ -2339,7 +2459,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>106</v>
@@ -2347,7 +2467,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>107</v>
@@ -2355,7 +2475,7 @@
     </row>
     <row r="112" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>108</v>
@@ -2363,7 +2483,7 @@
     </row>
     <row r="113" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>109</v>
@@ -2371,7 +2491,7 @@
     </row>
     <row r="114" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>140</v>
+        <v>169</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>110</v>
@@ -2379,7 +2499,7 @@
     </row>
     <row r="115" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>111</v>
@@ -2387,7 +2507,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>158</v>
+        <v>190</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>112</v>
@@ -2395,7 +2515,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>113</v>
@@ -2403,7 +2523,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>156</v>
+        <v>186</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>114</v>
@@ -2411,7 +2531,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>115</v>
@@ -2419,7 +2539,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>116</v>
@@ -2427,7 +2547,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>117</v>
@@ -2435,7 +2555,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>118</v>
@@ -2443,7 +2563,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>119</v>
@@ -2451,7 +2571,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>140</v>
+        <v>169</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>120</v>
@@ -2459,7 +2579,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>121</v>
@@ -2467,7 +2587,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>122</v>
@@ -2475,235 +2595,523 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>163</v>
+        <v>127</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B131" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>166</v>
+        <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>171</v>
+        <v>135</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>172</v>
+        <v>136</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>172</v>
+        <v>136</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>188</v>
+        <v>149</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>174</v>
+        <v>138</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>175</v>
+        <v>139</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>134</v>
+        <v>165</v>
       </c>
       <c r="B144" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="4" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>127</v>
-      </c>
-      <c r="B145" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>142</v>
-      </c>
-      <c r="B146" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+      <c r="B148" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B149" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B147" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    </row>
+    <row r="150" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A150" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A151" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A153" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A155" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A156" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B148" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>187</v>
-      </c>
-      <c r="B149" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>133</v>
-      </c>
-      <c r="B150" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>133</v>
-      </c>
-      <c r="B151" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>127</v>
-      </c>
-      <c r="B152" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>127</v>
-      </c>
-      <c r="B153" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154"/>
-      <c r="B154"/>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155"/>
-      <c r="B155"/>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156"/>
-      <c r="B156"/>
-    </row>
-    <row r="157" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157"/>
-      <c r="B157"/>
+      <c r="B167" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>214</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>